<commit_message>
Refonte de l'index, réglage de bugs sur la partie responsive.
</commit_message>
<xml_diff>
--- a/test_unitaire.xlsx
+++ b/test_unitaire.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="150" yWindow="630" windowWidth="21180" windowHeight="7620"/>
+    <workbookView xWindow="150" yWindow="630" windowWidth="21150" windowHeight="6900"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille 1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="53">
   <si>
     <t>Fichier JS</t>
   </si>
@@ -70,9 +70,6 @@
     <t>Il peut y avoir une erreur de type serveur (500) qui bloquera l'url et donc la empechera l'élément de s'afficher, alors on affichera un message de type "alert".</t>
   </si>
   <si>
-    <t>Il peut y avoir une erreur de type serveur (500) qui empechera de récuperer l'id du produit sélectionné précédament.</t>
-  </si>
-  <si>
     <t>17 à 34</t>
   </si>
   <si>
@@ -85,16 +82,10 @@
     <t>Cette fonction sert comme son nom l'indique à obtenir les élément du produit dans une URL (méthode get).</t>
   </si>
   <si>
-    <t>Cette fonction sert comme son nom l'indique à obtenir l'id  du produit dans une URL .</t>
-  </si>
-  <si>
     <t>On peut écrire le nom de la fonction en dehors d'elle-même pour afficher son contenue sur le document ou encore faire un console.log.</t>
   </si>
   <si>
     <t>Une erreur se produira si la fonction getItemByUrl est null. Ou encore si la "response" est mauvaise.</t>
-  </si>
-  <si>
-    <t>On peut tout simplement faire un console.log(data)</t>
   </si>
   <si>
     <t>38 à 133</t>
@@ -170,6 +161,18 @@
   </si>
   <si>
     <t>47 à 56</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Elle permet de calculer le prix totale des produits présents sur la page</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> console.log(data)</t>
+  </si>
+  <si>
+    <t>Il peut y avoir une erreur de type serveur (500) qui empechera de récuperer l'id du produit sélectionné précédament. L'utilisateur peu comprommettre la donnée en modifiant l'url.</t>
+  </si>
+  <si>
+    <t>Cette fonction sert à récuperer l'élément de l'api en passant par l'id récupéré dans la précédente fonction(getItemFromUrl).Et elle affiche ce produit dans le DOM en exécutant la fonction displayData.</t>
   </si>
 </sst>
 </file>
@@ -458,8 +461,8 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -531,7 +534,7 @@
         <v>9</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>10</v>
@@ -545,16 +548,16 @@
         <v>12</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="61.5" customHeight="1">
@@ -568,7 +571,7 @@
         <v>15</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>16</v>
@@ -582,19 +585,19 @@
         <v>11</v>
       </c>
       <c r="B6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>20</v>
-      </c>
       <c r="D6" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="61.5" customHeight="1">
@@ -602,139 +605,139 @@
         <v>11</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="61.5" customHeight="1">
       <c r="A8" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="8" t="s">
+      <c r="E8" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>36</v>
-      </c>
       <c r="F8" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="61.5" customHeight="1">
       <c r="A9" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B9" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="F9" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="61.5" customHeight="1">
       <c r="A10" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="61.5" customHeight="1">
       <c r="A11" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B11" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="7" t="s">
         <v>45</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="61.5" customHeight="1">
       <c r="A12" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C12" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>36</v>
-      </c>
       <c r="F12" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="61.5" customHeight="1">
       <c r="A13" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="61.5" customHeight="1">

</xml_diff>

<commit_message>
Rajout de fonctions sur le test unitaire
</commit_message>
<xml_diff>
--- a/test_unitaire.xlsx
+++ b/test_unitaire.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="57">
   <si>
     <t>Fichier JS</t>
   </si>
@@ -37,9 +37,6 @@
     <t>script.js</t>
   </si>
   <si>
-    <t>24 à 79</t>
-  </si>
-  <si>
     <t>displayData</t>
   </si>
   <si>
@@ -58,9 +55,6 @@
     <t>On peut vérifier cette fonction grâce au return searchParams.get('id'); ligne 6 qui permet tout simplement de récuperer l'élément sélectionné sur la page précédente envoyé par son id.</t>
   </si>
   <si>
-    <t>10 à 14</t>
-  </si>
-  <si>
     <t>displayError</t>
   </si>
   <si>
@@ -68,9 +62,6 @@
   </si>
   <si>
     <t>Il peut y avoir une erreur de type serveur (500) qui bloquera l'url et donc la empechera l'élément de s'afficher, alors on affichera un message de type "alert".</t>
-  </si>
-  <si>
-    <t>17 à 34</t>
   </si>
   <si>
     <t>getProductById</t>
@@ -86,9 +77,6 @@
   </si>
   <si>
     <t>Une erreur se produira si la fonction getItemByUrl est null. Ou encore si la "response" est mauvaise.</t>
-  </si>
-  <si>
-    <t>38 à 133</t>
   </si>
   <si>
     <t>Cette fonction sert à afficher les éléments du produits sélectionné sur la page précédente (_id, description, etc…)</t>
@@ -118,9 +106,6 @@
     <t>Tout simplement en écrivant le nom de la fonction en dehors des ses accolades ce qui fera normalement apparaitre son contenue sur le document html. On peut aussi utiliser le console.log.</t>
   </si>
   <si>
-    <t>91 à 99</t>
-  </si>
-  <si>
     <t>removeFromBasket</t>
   </si>
   <si>
@@ -139,12 +124,6 @@
     <t>calculTotalPriceProducts</t>
   </si>
   <si>
-    <t>Comme le nom l'indique, elle permet de calculer le prix totale des produits présents sur la page</t>
-  </si>
-  <si>
-    <t>131 à 186</t>
-  </si>
-  <si>
     <t>sendInfos</t>
   </si>
   <si>
@@ -152,15 +131,6 @@
   </si>
   <si>
     <t>Le contenue peut ne pas s'afficher par exemple à cause du erreur de syntaxe, ou encore à cause d'un élement non trouvé. On peut aussi avoir une erreur d'envoi au niveau de la requête.</t>
-  </si>
-  <si>
-    <t>validation.js</t>
-  </si>
-  <si>
-    <t>8 à 43</t>
-  </si>
-  <si>
-    <t>47 à 56</t>
   </si>
   <si>
     <t xml:space="preserve"> Elle permet de calculer le prix totale des produits présents sur la page</t>
@@ -173,6 +143,48 @@
   </si>
   <si>
     <t>Cette fonction sert à récuperer l'élément de l'api en passant par l'id récupéré dans la précédente fonction(getItemFromUrl).Et elle affiche ce produit dans le DOM en exécutant la fonction displayData.</t>
+  </si>
+  <si>
+    <t>101 à 119</t>
+  </si>
+  <si>
+    <t>123 à 133</t>
+  </si>
+  <si>
+    <t>calculQuantityProducts</t>
+  </si>
+  <si>
+    <t>On peu modifier cette quantitée depuis la page MVP d'un produit en ajoutant un nombre X de fois le produit dans le panier (et donc dans le localStorage), Ou alors directement depuis le panier en clicant "Retirer ce produit",</t>
+  </si>
+  <si>
+    <t>136 à 145</t>
+  </si>
+  <si>
+    <t>calculPriceProducts</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cette fonction permet de calculer la quantitée d'un produit ( tant bien sur le document que dans le localStorage )</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cette fonction permet de calculer le prix d'un produit ( tant bien sur le document que dans le localStorage )</t>
+  </si>
+  <si>
+    <t>On peu modifier ce prix depuis la page MVP d'un produit en ajoutant un nombre X de fois le produit dans le panier (et donc dans le localStorage). Ou alors directement depuis le panier en clicant "Retirer ce produit",</t>
+  </si>
+  <si>
+    <t>165 à 218</t>
+  </si>
+  <si>
+    <t>24 à 78</t>
+  </si>
+  <si>
+    <t>20 à 37</t>
+  </si>
+  <si>
+    <t>12 à 16</t>
+  </si>
+  <si>
+    <t>41 à 154</t>
   </si>
 </sst>
 </file>
@@ -461,8 +473,8 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -525,235 +537,237 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="61.5" customHeight="1">
       <c r="A4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="C4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>13</v>
-      </c>
       <c r="F4" s="7" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="61.5" customHeight="1">
       <c r="A5" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="F5" s="7" t="s">
         <v>15</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="61.5" customHeight="1">
       <c r="A6" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="C6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>22</v>
-      </c>
       <c r="F6" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="61.5" customHeight="1">
       <c r="A7" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="61.5" customHeight="1">
       <c r="A8" s="8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B8" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>33</v>
-      </c>
       <c r="F8" s="7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="61.5" customHeight="1">
       <c r="A9" s="8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="61.5" customHeight="1">
       <c r="A10" s="8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>49</v>
       </c>
       <c r="E10" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="7" t="s">
         <v>33</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="61.5" customHeight="1">
       <c r="A11" s="8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E11" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="7" t="s">
         <v>33</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="61.5" customHeight="1">
       <c r="A12" s="8" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="61.5" customHeight="1">
       <c r="A13" s="8" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="61.5" customHeight="1">
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-    </row>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="61.5" customHeight="1"/>
     <row r="15" spans="1:26" ht="61.5" customHeight="1">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
     </row>
     <row r="16" spans="1:26" ht="26.25" customHeight="1">
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
     </row>
     <row r="17" spans="4:6" ht="26.25" customHeight="1">
       <c r="D17" s="4"/>

</xml_diff>